<commit_message>
added temp graph to index
</commit_message>
<xml_diff>
--- a/data/Tipping Points Data.xlsx
+++ b/data/Tipping Points Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\freit\Documents\00 UniBremen\WS 18\Beyond Heatmaps\Project\FinalProject\D3Example\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3278B026-77FC-49DD-B294-A45E29396601}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C27311-EB2D-4D2D-AC33-ACC1E7C03ECE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -714,53 +714,11 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{7A2D7157-4AF2-4E63-894C-AA5D9F58603C}"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3230,15 +3188,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>4716780</xdr:colOff>
-      <xdr:row>213</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>899160</xdr:colOff>
-      <xdr:row>239</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>233</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3776,8 +3734,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="D240" sqref="D240"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="E215" sqref="E215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -8526,31 +8484,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:C204 B205:B209 C205:C272">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="between">
       <formula>3</formula>
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="between">
       <formula>1</formula>
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D210:D272">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="between">
       <formula>3</formula>
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="between">
       <formula>1</formula>
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B210:B272">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
       <formula>3</formula>
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
       <formula>1</formula>
       <formula>3</formula>
     </cfRule>

</xml_diff>

<commit_message>
added stabilised data. updated main structure
</commit_message>
<xml_diff>
--- a/data/Tipping Points Data.xlsx
+++ b/data/Tipping Points Data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\freit\Documents\00 UniBremen\WS 18\Beyond Heatmaps\Project\FinalProject\D3Example\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C27311-EB2D-4D2D-AC33-ACC1E7C03ECE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E55A02-21C2-4577-9C6C-D896CD970E43}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Processes" sheetId="1" r:id="rId1"/>
-    <sheet name="Temperatures" sheetId="5" r:id="rId2"/>
-    <sheet name="Folha4" sheetId="2" r:id="rId3"/>
-    <sheet name="Feedbacks" sheetId="3" r:id="rId4"/>
-    <sheet name="Temperatures simulation" sheetId="6" r:id="rId5"/>
+    <sheet name="Temp - HotHouse" sheetId="5" r:id="rId2"/>
+    <sheet name="Temp - Stabilised" sheetId="7" r:id="rId3"/>
+    <sheet name="Folha4" sheetId="2" r:id="rId4"/>
+    <sheet name="Feedbacks" sheetId="3" r:id="rId5"/>
+    <sheet name="Temperatures simulation" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="131">
   <si>
     <t>Process</t>
   </si>
@@ -807,7 +808,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Temperatures!$B$1</c:f>
+              <c:f>'Temp - HotHouse'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -830,7 +831,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Temperatures!$A$2:$A$272</c:f>
+              <c:f>'Temp - HotHouse'!$A$2:$A$272</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="271"/>
@@ -1652,7 +1653,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Temperatures!$B$2:$B$272</c:f>
+              <c:f>'Temp - HotHouse'!$B$2:$B$272</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="271"/>
@@ -2627,6 +2628,1057 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Temp - Stabilised'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Annomaly</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Temp - Stabilised'!$A$2:$A$132</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="131"/>
+                <c:pt idx="0">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2051</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2052</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2053</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2054</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2055</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2056</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2057</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2058</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2059</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2060</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2061</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2062</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2063</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2064</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2065</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2066</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2067</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2068</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2069</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2070</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2071</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2072</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2073</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2074</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2075</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2076</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2077</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2078</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2079</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2080</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2081</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2082</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2083</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2084</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2085</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2086</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2087</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2088</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2089</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2090</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2091</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2092</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2093</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2094</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2095</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2096</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2097</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2098</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2099</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2101</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2102</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2103</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2104</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2105</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2106</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2107</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2108</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2109</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2110</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2111</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2112</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2113</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2114</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2115</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2116</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2117</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2118</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2119</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2120</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2121</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2122</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2123</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2124</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>2125</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>2126</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>2127</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>2128</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>2129</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>2130</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>2131</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>2132</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>2133</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>2134</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>2135</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>2136</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>2137</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>2138</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>2139</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>2140</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>2141</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>2142</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>2143</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>2144</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>2145</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>2146</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>2147</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>2148</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>2149</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>2150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Temp - Stabilised'!$B$2:$B$132</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="131"/>
+                <c:pt idx="0">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.41</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.43</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.44</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.46</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.46</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.47</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.49</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.49</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.49</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.47</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.47</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.46</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.46</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.46</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.44</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.43</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.43</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.42</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.41</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.39</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.39</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.37</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.36</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.36</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.34</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.34</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.33</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.32</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.32</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.31</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.31</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.29</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.29</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.28</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.26</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.26</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.24</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.24</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.24</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.24</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.24</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.23</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.23</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.23</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.23</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.23</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.23</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.23</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.23</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.23</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.23</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1.19</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1.17</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F39B-406A-8CF6-1E1604FA82F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="529695848"/>
+        <c:axId val="529690928"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="529695848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="529690928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="529690928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="529695848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2667,7 +3719,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3226,6 +4834,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BD220B6-4EC3-4B36-8B12-62E704331DEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3734,8 +5383,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="E215" sqref="E215"/>
+    <sheetView topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -8529,6 +10178,1081 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A261A8A-B6A8-4C73-828C-146C95C26EF1}">
+  <dimension ref="A1:B132"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection sqref="A1:B132"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="29">
+        <v>2020</v>
+      </c>
+      <c r="B2" s="29">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="29">
+        <v>2021</v>
+      </c>
+      <c r="B3" s="29">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="29">
+        <v>2022</v>
+      </c>
+      <c r="B4" s="29">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="29">
+        <v>2023</v>
+      </c>
+      <c r="B5" s="29">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="29">
+        <v>2024</v>
+      </c>
+      <c r="B6" s="29">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="29">
+        <v>2025</v>
+      </c>
+      <c r="B7" s="29">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="29">
+        <v>2026</v>
+      </c>
+      <c r="B8" s="29">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="29">
+        <v>2027</v>
+      </c>
+      <c r="B9" s="29">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="29">
+        <v>2028</v>
+      </c>
+      <c r="B10" s="29">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="29">
+        <v>2029</v>
+      </c>
+      <c r="B11" s="29">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="29">
+        <v>2030</v>
+      </c>
+      <c r="B12" s="29">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="29">
+        <v>2031</v>
+      </c>
+      <c r="B13" s="29">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="29">
+        <v>2032</v>
+      </c>
+      <c r="B14" s="29">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="29">
+        <v>2033</v>
+      </c>
+      <c r="B15" s="29">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="29">
+        <v>2034</v>
+      </c>
+      <c r="B16" s="29">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="29">
+        <v>2035</v>
+      </c>
+      <c r="B17" s="29">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="29">
+        <v>2036</v>
+      </c>
+      <c r="B18" s="29">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="29">
+        <v>2037</v>
+      </c>
+      <c r="B19" s="29">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="29">
+        <v>2038</v>
+      </c>
+      <c r="B20" s="29">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="29">
+        <v>2039</v>
+      </c>
+      <c r="B21" s="29">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="29">
+        <v>2040</v>
+      </c>
+      <c r="B22" s="29">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="29">
+        <v>2041</v>
+      </c>
+      <c r="B23" s="29">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="29">
+        <v>2042</v>
+      </c>
+      <c r="B24" s="29">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="29">
+        <v>2043</v>
+      </c>
+      <c r="B25" s="29">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="29">
+        <v>2044</v>
+      </c>
+      <c r="B26" s="29">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="29">
+        <v>2045</v>
+      </c>
+      <c r="B27" s="29">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="29">
+        <v>2046</v>
+      </c>
+      <c r="B28" s="29">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="29">
+        <v>2047</v>
+      </c>
+      <c r="B29" s="29">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="29">
+        <v>2048</v>
+      </c>
+      <c r="B30" s="29">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="29">
+        <v>2049</v>
+      </c>
+      <c r="B31" s="29">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="29">
+        <v>2050</v>
+      </c>
+      <c r="B32" s="29">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="29">
+        <v>2051</v>
+      </c>
+      <c r="B33" s="29">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="29">
+        <v>2052</v>
+      </c>
+      <c r="B34" s="29">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="29">
+        <v>2053</v>
+      </c>
+      <c r="B35" s="29">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="29">
+        <v>2054</v>
+      </c>
+      <c r="B36" s="29">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="29">
+        <v>2055</v>
+      </c>
+      <c r="B37" s="29">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="29">
+        <v>2056</v>
+      </c>
+      <c r="B38" s="29">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="29">
+        <v>2057</v>
+      </c>
+      <c r="B39" s="29">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="29">
+        <v>2058</v>
+      </c>
+      <c r="B40" s="29">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="29">
+        <v>2059</v>
+      </c>
+      <c r="B41" s="29">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="29">
+        <v>2060</v>
+      </c>
+      <c r="B42" s="29">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="29">
+        <v>2061</v>
+      </c>
+      <c r="B43" s="29">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="29">
+        <v>2062</v>
+      </c>
+      <c r="B44" s="29">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="29">
+        <v>2063</v>
+      </c>
+      <c r="B45" s="29">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="29">
+        <v>2064</v>
+      </c>
+      <c r="B46" s="29">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="29">
+        <v>2065</v>
+      </c>
+      <c r="B47" s="29">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="29">
+        <v>2066</v>
+      </c>
+      <c r="B48" s="29">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="29">
+        <v>2067</v>
+      </c>
+      <c r="B49" s="29">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="29">
+        <v>2068</v>
+      </c>
+      <c r="B50" s="29">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="29">
+        <v>2069</v>
+      </c>
+      <c r="B51" s="29">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="29">
+        <v>2070</v>
+      </c>
+      <c r="B52" s="29">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="29">
+        <v>2071</v>
+      </c>
+      <c r="B53" s="29">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="29">
+        <v>2072</v>
+      </c>
+      <c r="B54" s="29">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="29">
+        <v>2073</v>
+      </c>
+      <c r="B55" s="29">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="29">
+        <v>2074</v>
+      </c>
+      <c r="B56" s="29">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="29">
+        <v>2075</v>
+      </c>
+      <c r="B57" s="29">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="29">
+        <v>2076</v>
+      </c>
+      <c r="B58" s="29">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="29">
+        <v>2077</v>
+      </c>
+      <c r="B59" s="29">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="29">
+        <v>2078</v>
+      </c>
+      <c r="B60" s="29">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="29">
+        <v>2079</v>
+      </c>
+      <c r="B61" s="29">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="29">
+        <v>2080</v>
+      </c>
+      <c r="B62" s="29">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="29">
+        <v>2081</v>
+      </c>
+      <c r="B63" s="29">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="29">
+        <v>2082</v>
+      </c>
+      <c r="B64" s="29">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="29">
+        <v>2083</v>
+      </c>
+      <c r="B65" s="29">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="29">
+        <v>2084</v>
+      </c>
+      <c r="B66" s="29">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="29">
+        <v>2085</v>
+      </c>
+      <c r="B67" s="29">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="29">
+        <v>2086</v>
+      </c>
+      <c r="B68" s="29">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="29">
+        <v>2087</v>
+      </c>
+      <c r="B69" s="29">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="29">
+        <v>2088</v>
+      </c>
+      <c r="B70" s="29">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="29">
+        <v>2089</v>
+      </c>
+      <c r="B71" s="29">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="29">
+        <v>2090</v>
+      </c>
+      <c r="B72" s="29">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="29">
+        <v>2091</v>
+      </c>
+      <c r="B73" s="29">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="29">
+        <v>2092</v>
+      </c>
+      <c r="B74" s="29">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="29">
+        <v>2093</v>
+      </c>
+      <c r="B75" s="29">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="29">
+        <v>2094</v>
+      </c>
+      <c r="B76" s="29">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="29">
+        <v>2095</v>
+      </c>
+      <c r="B77" s="29">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="29">
+        <v>2096</v>
+      </c>
+      <c r="B78" s="29">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="29">
+        <v>2097</v>
+      </c>
+      <c r="B79" s="29">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="29">
+        <v>2098</v>
+      </c>
+      <c r="B80" s="29">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="29">
+        <v>2099</v>
+      </c>
+      <c r="B81" s="29">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="29">
+        <v>2100</v>
+      </c>
+      <c r="B82" s="29">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="29">
+        <v>2101</v>
+      </c>
+      <c r="B83" s="29">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="29">
+        <v>2102</v>
+      </c>
+      <c r="B84" s="29">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="29">
+        <v>2103</v>
+      </c>
+      <c r="B85" s="29">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="29">
+        <v>2104</v>
+      </c>
+      <c r="B86" s="29">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="29">
+        <v>2105</v>
+      </c>
+      <c r="B87" s="29">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="29">
+        <v>2106</v>
+      </c>
+      <c r="B88" s="29">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="29">
+        <v>2107</v>
+      </c>
+      <c r="B89" s="29">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="29">
+        <v>2108</v>
+      </c>
+      <c r="B90" s="29">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="29">
+        <v>2109</v>
+      </c>
+      <c r="B91" s="29">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="29">
+        <v>2110</v>
+      </c>
+      <c r="B92" s="29">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="29">
+        <v>2111</v>
+      </c>
+      <c r="B93" s="29">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="29">
+        <v>2112</v>
+      </c>
+      <c r="B94" s="29">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="29">
+        <v>2113</v>
+      </c>
+      <c r="B95" s="29">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="29">
+        <v>2114</v>
+      </c>
+      <c r="B96" s="29">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="29">
+        <v>2115</v>
+      </c>
+      <c r="B97" s="29">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="29">
+        <v>2116</v>
+      </c>
+      <c r="B98" s="29">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="29">
+        <v>2117</v>
+      </c>
+      <c r="B99" s="29">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="29">
+        <v>2118</v>
+      </c>
+      <c r="B100" s="29">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="29">
+        <v>2119</v>
+      </c>
+      <c r="B101" s="29">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="29">
+        <v>2120</v>
+      </c>
+      <c r="B102" s="29">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="29">
+        <v>2121</v>
+      </c>
+      <c r="B103" s="29">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="29">
+        <v>2122</v>
+      </c>
+      <c r="B104" s="29">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="29">
+        <v>2123</v>
+      </c>
+      <c r="B105" s="29">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="29">
+        <v>2124</v>
+      </c>
+      <c r="B106" s="29">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="29">
+        <v>2125</v>
+      </c>
+      <c r="B107" s="29">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="29">
+        <v>2126</v>
+      </c>
+      <c r="B108" s="29">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="29">
+        <v>2127</v>
+      </c>
+      <c r="B109" s="29">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="29">
+        <v>2128</v>
+      </c>
+      <c r="B110" s="29">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="29">
+        <v>2129</v>
+      </c>
+      <c r="B111" s="29">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="29">
+        <v>2130</v>
+      </c>
+      <c r="B112" s="29">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="29">
+        <v>2131</v>
+      </c>
+      <c r="B113" s="29">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="29">
+        <v>2132</v>
+      </c>
+      <c r="B114" s="29">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="29">
+        <v>2133</v>
+      </c>
+      <c r="B115" s="29">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="29">
+        <v>2134</v>
+      </c>
+      <c r="B116" s="29">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="29">
+        <v>2135</v>
+      </c>
+      <c r="B117" s="29">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="29">
+        <v>2136</v>
+      </c>
+      <c r="B118" s="29">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="29">
+        <v>2137</v>
+      </c>
+      <c r="B119" s="29">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="29">
+        <v>2138</v>
+      </c>
+      <c r="B120" s="29">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="29">
+        <v>2139</v>
+      </c>
+      <c r="B121" s="29">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="29">
+        <v>2140</v>
+      </c>
+      <c r="B122" s="29">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="29">
+        <v>2141</v>
+      </c>
+      <c r="B123" s="29">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="29">
+        <v>2142</v>
+      </c>
+      <c r="B124" s="29">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="29">
+        <v>2143</v>
+      </c>
+      <c r="B125" s="29">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="29">
+        <v>2144</v>
+      </c>
+      <c r="B126" s="29">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="29">
+        <v>2145</v>
+      </c>
+      <c r="B127" s="29">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="29">
+        <v>2146</v>
+      </c>
+      <c r="B128" s="29">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="29">
+        <v>2147</v>
+      </c>
+      <c r="B129" s="29">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="29">
+        <v>2148</v>
+      </c>
+      <c r="B130" s="29">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="29">
+        <v>2149</v>
+      </c>
+      <c r="B131" s="29">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="29">
+        <v>2150</v>
+      </c>
+      <c r="B132" s="29">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -8941,7 +11665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -9064,7 +11788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
adapted texts and fixed an issue with (dis)apparition of navigation dots on refresh
</commit_message>
<xml_diff>
--- a/data/Tipping Points Data.xlsx
+++ b/data/Tipping Points Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\freit\Documents\00 UniBremen\WS 18\Beyond Heatmaps\Project\FinalProject\D3Example\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yjenn\Documents\Uni\Uni Bremen\HFK\BeyondHeatmaps\project\gitRepoVS\D3Example\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E55A02-21C2-4577-9C6C-D896CD970E43}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68D8AE0-BE52-42F7-89C9-9560EC9B8D0B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Processes" sheetId="1" r:id="rId1"/>
@@ -712,8 +712,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{7A2D7157-4AF2-4E63-894C-AA5D9F58603C}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -786,7 +786,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2545,7 +2545,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="522688904"/>
@@ -2587,7 +2587,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2617,7 +2617,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2631,7 +2631,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2668,7 +2668,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3568,7 +3568,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="529690928"/>
@@ -3627,7 +3627,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="529695848"/>
@@ -3668,7 +3668,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4876,7 +4876,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5181,7 +5181,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="23.88671875" customWidth="1"/>
     <col min="2" max="3" width="20.109375" customWidth="1"/>
@@ -5383,11 +5383,11 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="B146" sqref="B146"/>
+    <sheetView tabSelected="1" topLeftCell="A234" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D247" sqref="D247"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="4" max="4" width="72.88671875" customWidth="1"/>
     <col min="5" max="5" width="56" customWidth="1"/>
@@ -7695,7 +7695,6 @@
         <v>6.1199999999999983</v>
       </c>
       <c r="C247" s="29"/>
-      <c r="D247" s="29"/>
     </row>
     <row r="248" spans="1:4" ht="13.2">
       <c r="A248" s="14">
@@ -10142,7 +10141,7 @@
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D210:D272">
+  <conditionalFormatting sqref="D210:D246 D248:D272">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="between">
       <formula>3</formula>
       <formula>5</formula>
@@ -10181,11 +10180,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A261A8A-B6A8-4C73-828C-146C95C26EF1}">
   <dimension ref="A1:B132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="2" width="8.88671875" style="29"/>
   </cols>
@@ -11263,7 +11262,7 @@
       <selection activeCell="A5" sqref="A5:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="44.88671875" customWidth="1"/>
     <col min="2" max="2" width="20.5546875" customWidth="1"/>
@@ -11674,7 +11673,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
     <col min="2" max="2" width="23.88671875" customWidth="1"/>
@@ -11795,11 +11794,11 @@
   </sheetPr>
   <dimension ref="A1:E1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="3" width="14.44140625" style="29"/>
   </cols>

</xml_diff>